<commit_message>
Matching 3 pre-control indicators
</commit_message>
<xml_diff>
--- a/Zetas_new.xlsx
+++ b/Zetas_new.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Z541213\Documents\Project\Model\Schisto_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11A98D5D-294D-4582-9FED-892124FDB45C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F0DE19-84E2-4B65-9CA2-3DAF6BD1D2BF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="14">
   <si>
     <t xml:space="preserve">Endemicity </t>
   </si>
@@ -77,17 +77,14 @@
   <si>
     <t>Transmission on snails</t>
   </si>
-  <si>
-    <t>Ext Foi can be lowered even more to achieve faster the equilibrium</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0E+00"/>
+    <numFmt numFmtId="167" formatCode="0.0E+00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -226,7 +223,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -267,18 +264,16 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -562,8 +557,8 @@
   <dimension ref="A1:XFC76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1093,7 +1088,7 @@
       <c r="G20" s="16">
         <v>0.1</v>
       </c>
-      <c r="H20" s="49">
+      <c r="H20" s="41">
         <v>3E-10</v>
       </c>
     </row>
@@ -1119,7 +1114,7 @@
       <c r="G21" s="16">
         <v>0.1</v>
       </c>
-      <c r="H21" s="49">
+      <c r="H21" s="41">
         <v>4.0000000000000001E-10</v>
       </c>
     </row>
@@ -1145,7 +1140,7 @@
       <c r="G22" s="16">
         <v>0.1</v>
       </c>
-      <c r="H22" s="49">
+      <c r="H22" s="41">
         <v>4.0000000000000001E-10</v>
       </c>
     </row>
@@ -1171,7 +1166,7 @@
       <c r="G23" s="18">
         <v>0.1</v>
       </c>
-      <c r="H23" s="50">
+      <c r="H23" s="42">
         <v>3E-10</v>
       </c>
     </row>
@@ -1197,7 +1192,7 @@
       <c r="G24" s="18">
         <v>0.1</v>
       </c>
-      <c r="H24" s="50">
+      <c r="H24" s="42">
         <v>4.0000000000000001E-10</v>
       </c>
     </row>
@@ -1223,7 +1218,7 @@
       <c r="G25" s="18">
         <v>0.1</v>
       </c>
-      <c r="H25" s="50">
+      <c r="H25" s="42">
         <v>4.0000000000000001E-10</v>
       </c>
     </row>
@@ -1249,7 +1244,7 @@
       <c r="G26" s="20">
         <v>0.05</v>
       </c>
-      <c r="H26" s="48">
+      <c r="H26" s="40">
         <v>2.0000000000000001E-10</v>
       </c>
     </row>
@@ -1275,7 +1270,7 @@
       <c r="G27" s="20">
         <v>0.05</v>
       </c>
-      <c r="H27" s="48">
+      <c r="H27" s="40">
         <v>3E-10</v>
       </c>
     </row>
@@ -1301,7 +1296,7 @@
       <c r="G28" s="26">
         <v>0.05</v>
       </c>
-      <c r="H28" s="51">
+      <c r="H28" s="43">
         <v>3E-10</v>
       </c>
     </row>
@@ -1348,7 +1343,7 @@
         <v>0</v>
       </c>
       <c r="F30" s="4">
-        <v>1.6437790000000001E-4</v>
+        <v>1.65E-4</v>
       </c>
       <c r="G30" s="4">
         <v>0.2</v>
@@ -1374,7 +1369,7 @@
         <v>0</v>
       </c>
       <c r="F31" s="4">
-        <v>1.6437790000000001E-4</v>
+        <v>1.65E-4</v>
       </c>
       <c r="G31" s="4">
         <v>0.2</v>
@@ -1426,7 +1421,7 @@
         <v>0</v>
       </c>
       <c r="F33" s="6">
-        <v>1.6899999999999999E-4</v>
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="G33" s="6">
         <v>0.2</v>
@@ -1452,7 +1447,7 @@
         <v>0</v>
       </c>
       <c r="F34" s="6">
-        <v>1.6899999999999999E-4</v>
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="G34" s="6">
         <v>0.2</v>
@@ -1637,7 +1632,7 @@
         <v>0.09</v>
       </c>
       <c r="F41" s="12">
-        <v>0.16200000000000001</v>
+        <v>0.16400000000000001</v>
       </c>
       <c r="G41" s="12">
         <v>0.18</v>
@@ -1660,13 +1655,13 @@
         <v>6</v>
       </c>
       <c r="E42" s="13">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="F42" s="12">
-        <v>8.7999999999999995E-2</v>
+        <v>0.15</v>
       </c>
       <c r="G42" s="12">
-        <v>0.2</v>
+        <v>0.18</v>
       </c>
       <c r="H42" s="12">
         <v>1E-10</v>
@@ -1686,13 +1681,13 @@
         <v>7</v>
       </c>
       <c r="E43" s="13">
-        <v>7.0000000000000007E-2</v>
+        <v>0.1</v>
       </c>
       <c r="F43" s="12">
-        <v>8.7999999999999995E-2</v>
+        <v>0.15</v>
       </c>
       <c r="G43" s="12">
-        <v>0.2</v>
+        <v>0.18</v>
       </c>
       <c r="H43" s="12">
         <v>1E-10</v>
@@ -1712,7 +1707,7 @@
         <v>5</v>
       </c>
       <c r="E44" s="15">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="F44" s="14">
         <v>5</v>
@@ -1721,7 +1716,7 @@
         <v>0.1</v>
       </c>
       <c r="H44" s="14">
-        <v>1E-10</v>
+        <v>6E-11</v>
       </c>
     </row>
     <row r="45" spans="1:16383" s="14" customFormat="1" x14ac:dyDescent="0.3">
@@ -1738,7 +1733,7 @@
         <v>6</v>
       </c>
       <c r="E45" s="15">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="F45" s="14">
         <v>5</v>
@@ -50993,16 +50988,16 @@
         <v>5</v>
       </c>
       <c r="E50" s="19">
-        <v>7.0000000000000007E-2</v>
+        <v>0.1</v>
       </c>
       <c r="F50" s="18">
-        <v>0.14799999999999999</v>
+        <v>0.27</v>
       </c>
       <c r="G50" s="18">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="H50" s="18">
-        <v>1E-10</v>
+        <v>7.0000000000000004E-11</v>
       </c>
     </row>
     <row r="51" spans="1:16383" x14ac:dyDescent="0.3">
@@ -51019,16 +51014,16 @@
         <v>6</v>
       </c>
       <c r="E51" s="19">
-        <v>7.0000000000000007E-2</v>
+        <v>0.1</v>
       </c>
       <c r="F51" s="18">
-        <v>0.14799999999999999</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G51" s="18">
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
       <c r="H51" s="18">
-        <v>1E-10</v>
+        <v>8.9999999999999999E-11</v>
       </c>
     </row>
     <row r="52" spans="1:16383" x14ac:dyDescent="0.3">
@@ -51045,16 +51040,16 @@
         <v>7</v>
       </c>
       <c r="E52" s="19">
-        <v>7.0000000000000007E-2</v>
+        <v>0.1</v>
       </c>
       <c r="F52" s="18">
-        <v>0.14799999999999999</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G52" s="18">
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
       <c r="H52" s="18">
-        <v>1E-10</v>
+        <v>8.9999999999999999E-11</v>
       </c>
     </row>
     <row r="53" spans="1:16383" x14ac:dyDescent="0.3">
@@ -51071,16 +51066,16 @@
         <v>5</v>
       </c>
       <c r="E53" s="21">
+        <v>0.11</v>
+      </c>
+      <c r="F53" s="20">
+        <v>9</v>
+      </c>
+      <c r="G53" s="20">
         <v>0.1</v>
       </c>
-      <c r="F53" s="20">
-        <v>0.08</v>
-      </c>
-      <c r="G53" s="20">
-        <v>0.3</v>
-      </c>
-      <c r="H53" s="48">
-        <v>3E-10</v>
+      <c r="H53" s="40">
+        <v>7.0000000000000004E-11</v>
       </c>
     </row>
     <row r="54" spans="1:16383" x14ac:dyDescent="0.3">
@@ -51100,13 +51095,13 @@
         <v>0.1</v>
       </c>
       <c r="F54" s="20">
-        <v>0.08</v>
+        <v>8</v>
       </c>
       <c r="G54" s="20">
-        <v>0.3</v>
-      </c>
-      <c r="H54" s="48">
-        <v>3E-10</v>
+        <v>0.1</v>
+      </c>
+      <c r="H54" s="40">
+        <v>1E-10</v>
       </c>
     </row>
     <row r="55" spans="1:16383" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -51126,13 +51121,13 @@
         <v>0.1</v>
       </c>
       <c r="F55" s="26">
-        <v>0.08</v>
+        <v>8</v>
       </c>
       <c r="G55" s="26">
-        <v>0.3</v>
-      </c>
-      <c r="H55" s="51">
-        <v>3E-10</v>
+        <v>0.1</v>
+      </c>
+      <c r="H55" s="43">
+        <v>1E-10</v>
       </c>
     </row>
     <row r="56" spans="1:16383" x14ac:dyDescent="0.3">
@@ -51226,21 +51221,17 @@
       <c r="D59" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E59" s="44">
-        <v>3.0000000000000001E-3</v>
+      <c r="E59" s="11">
+        <v>0.1</v>
       </c>
       <c r="F59" s="10">
-        <v>3.4500000000000003E-2</v>
+        <v>8.9999999999999998E-4</v>
       </c>
       <c r="G59" s="10">
-        <v>0.1</v>
-      </c>
-      <c r="H59" s="10">
-        <f>10^(-10)</f>
-        <v>1E-10</v>
-      </c>
-      <c r="I59" s="10" t="s">
-        <v>14</v>
+        <v>0.05</v>
+      </c>
+      <c r="H59" s="44">
+        <v>4.8E-9</v>
       </c>
     </row>
     <row r="60" spans="1:16383" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -51256,18 +51247,17 @@
       <c r="D60" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E60" s="44">
-        <v>3.0000000000000001E-3</v>
+      <c r="E60" s="11">
+        <v>0.1</v>
       </c>
       <c r="F60" s="10">
-        <v>3.4500000000000003E-2</v>
+        <v>8.9999999999999998E-4</v>
       </c>
       <c r="G60" s="10">
-        <v>0.1</v>
-      </c>
-      <c r="H60" s="10">
-        <f t="shared" ref="H60:H61" si="2">10^(-10)</f>
-        <v>1E-10</v>
+        <v>0.05</v>
+      </c>
+      <c r="H60" s="45">
+        <v>5.0000000000000001E-9</v>
       </c>
     </row>
     <row r="61" spans="1:16383" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -51283,18 +51273,17 @@
       <c r="D61" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E61" s="44">
-        <v>2E-3</v>
+      <c r="E61" s="11">
+        <v>0.1</v>
       </c>
       <c r="F61" s="10">
-        <v>3.4500000000000003E-2</v>
+        <v>8.9999999999999998E-4</v>
       </c>
       <c r="G61" s="10">
-        <v>0.1</v>
-      </c>
-      <c r="H61" s="10">
-        <f t="shared" si="2"/>
-        <v>1E-10</v>
+        <v>0.05</v>
+      </c>
+      <c r="H61" s="45">
+        <v>5.0000000000000001E-9</v>
       </c>
     </row>
     <row r="62" spans="1:16383" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -51310,17 +51299,17 @@
       <c r="D62" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E62" s="45">
-        <v>2E-3</v>
+      <c r="E62" s="13">
+        <v>0.1</v>
       </c>
       <c r="F62" s="12">
-        <v>3.5000000000000003E-2</v>
+        <v>8.9999999999999998E-4</v>
       </c>
       <c r="G62" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="H62" s="12">
-        <v>1E-10</v>
+        <v>0.05</v>
+      </c>
+      <c r="H62" s="46">
+        <v>5.0000000000000001E-9</v>
       </c>
     </row>
     <row r="63" spans="1:16383" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -51336,17 +51325,17 @@
       <c r="D63" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E63" s="45">
-        <v>1E-3</v>
+      <c r="E63" s="13">
+        <v>0.1</v>
       </c>
       <c r="F63" s="12">
-        <v>3.5000000000000003E-2</v>
+        <v>8.9999999999999998E-4</v>
       </c>
       <c r="G63" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="H63" s="12">
-        <v>1E-10</v>
+        <v>0.05</v>
+      </c>
+      <c r="H63" s="46">
+        <v>5.0000000000000001E-9</v>
       </c>
     </row>
     <row r="64" spans="1:16383" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -51362,17 +51351,17 @@
       <c r="D64" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E64" s="45">
-        <v>1E-3</v>
+      <c r="E64" s="13">
+        <v>0.09</v>
       </c>
       <c r="F64" s="12">
-        <v>3.5000000000000003E-2</v>
+        <v>8.9999999999999998E-4</v>
       </c>
       <c r="G64" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="H64" s="12">
-        <v>1E-10</v>
+        <v>0.05</v>
+      </c>
+      <c r="H64" s="46">
+        <v>5.0000000000000001E-9</v>
       </c>
     </row>
     <row r="65" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.3">
@@ -51388,17 +51377,17 @@
       <c r="D65" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E65" s="43">
-        <v>4.0000000000000001E-3</v>
+      <c r="E65" s="15">
+        <v>0.09</v>
       </c>
       <c r="F65" s="14">
-        <v>0.02</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="G65" s="14">
-        <v>0.1</v>
-      </c>
-      <c r="H65" s="14">
-        <v>2.0000000000000001E-10</v>
+        <v>0.05</v>
+      </c>
+      <c r="H65" s="47">
+        <v>5.0000000000000001E-9</v>
       </c>
     </row>
     <row r="66" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.3">
@@ -51414,17 +51403,17 @@
       <c r="D66" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E66" s="43">
-        <v>4.0000000000000001E-3</v>
+      <c r="E66" s="15">
+        <v>0.09</v>
       </c>
       <c r="F66" s="14">
-        <v>0.02</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="G66" s="14">
-        <v>0.1</v>
-      </c>
-      <c r="H66" s="14">
-        <v>2.0000000000000001E-10</v>
+        <v>0.05</v>
+      </c>
+      <c r="H66" s="47">
+        <v>5.0000000000000001E-9</v>
       </c>
     </row>
     <row r="67" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.3">
@@ -51440,17 +51429,17 @@
       <c r="D67" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E67" s="43">
-        <v>4.0000000000000001E-3</v>
+      <c r="E67" s="15">
+        <v>0.09</v>
       </c>
       <c r="F67" s="14">
-        <v>0.02</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="G67" s="14">
-        <v>0.1</v>
-      </c>
-      <c r="H67" s="14">
-        <v>2.0000000000000001E-10</v>
+        <v>0.05</v>
+      </c>
+      <c r="H67" s="47">
+        <v>5.0000000000000001E-9</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
@@ -51466,17 +51455,17 @@
       <c r="D68" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E68" s="40">
-        <v>3.0000000000000001E-3</v>
+      <c r="E68" s="25">
+        <v>0.1</v>
       </c>
       <c r="F68" s="24">
-        <v>7.1999999999999998E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="G68" s="24">
-        <v>0.1</v>
-      </c>
-      <c r="H68" s="49">
-        <v>1.0000000000000001E-9</v>
+        <v>0.05</v>
+      </c>
+      <c r="H68" s="48">
+        <v>4.4999999999999998E-9</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.3">
@@ -51492,17 +51481,17 @@
       <c r="D69" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="E69" s="41">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="F69" s="16">
-        <v>7.1999999999999998E-3</v>
+      <c r="E69" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="F69" s="24">
+        <v>2E-3</v>
       </c>
       <c r="G69" s="24">
-        <v>0.1</v>
-      </c>
-      <c r="H69" s="49">
-        <v>1.0000000000000001E-9</v>
+        <v>0.05</v>
+      </c>
+      <c r="H69" s="48">
+        <v>4.4999999999999998E-9</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
@@ -51518,17 +51507,17 @@
       <c r="D70" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="E70" s="40">
-        <v>6.0000000000000001E-3</v>
+      <c r="E70" s="25">
+        <v>0.1</v>
       </c>
       <c r="F70" s="24">
-        <v>7.1999999999999998E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="G70" s="24">
-        <v>0.1</v>
-      </c>
-      <c r="H70" s="49">
-        <v>1.0000000000000001E-9</v>
+        <v>0.05</v>
+      </c>
+      <c r="H70" s="48">
+        <v>4.4999999999999998E-9</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.3">
@@ -51544,17 +51533,17 @@
       <c r="D71" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="E71" s="42">
+      <c r="E71" s="19">
+        <v>0.09</v>
+      </c>
+      <c r="F71" s="18">
         <v>2E-3</v>
       </c>
-      <c r="F71" s="18">
-        <v>7.1999999999999998E-3</v>
-      </c>
       <c r="G71" s="18">
-        <v>0.1</v>
-      </c>
-      <c r="H71" s="50">
-        <v>1.0000000000000001E-9</v>
+        <v>0.05</v>
+      </c>
+      <c r="H71" s="49">
+        <v>4.4999999999999998E-9</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.3">
@@ -51570,17 +51559,17 @@
       <c r="D72" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="E72" s="42">
-        <v>3.0000000000000001E-3</v>
+      <c r="E72" s="19">
+        <v>0.09</v>
       </c>
       <c r="F72" s="18">
-        <v>7.1999999999999998E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="G72" s="18">
-        <v>0.1</v>
-      </c>
-      <c r="H72" s="50">
-        <v>1.0000000000000001E-9</v>
+        <v>0.05</v>
+      </c>
+      <c r="H72" s="49">
+        <v>4.4999999999999998E-9</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.3">
@@ -51596,17 +51585,17 @@
       <c r="D73" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="E73" s="42">
-        <v>4.0000000000000001E-3</v>
+      <c r="E73" s="19">
+        <v>0.09</v>
       </c>
       <c r="F73" s="18">
-        <v>7.1999999999999998E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="G73" s="18">
-        <v>0.1</v>
-      </c>
-      <c r="H73" s="50">
-        <v>1.0000000000000001E-9</v>
+        <v>0.05</v>
+      </c>
+      <c r="H73" s="49">
+        <v>4.4999999999999998E-9</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.3">
@@ -51622,17 +51611,17 @@
       <c r="D74" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E74" s="46">
-        <v>4.0000000000000001E-3</v>
+      <c r="E74" s="21">
+        <v>0.09</v>
       </c>
       <c r="F74" s="20">
-        <v>3.9E-2</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="G74" s="20">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="H74" s="20">
-        <v>2.0000000000000001E-10</v>
+        <v>4.4999999999999998E-9</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.3">
@@ -51648,17 +51637,17 @@
       <c r="D75" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="E75" s="46">
-        <v>4.0000000000000001E-3</v>
+      <c r="E75" s="21">
+        <v>0.09</v>
       </c>
       <c r="F75" s="20">
-        <v>3.9E-2</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="G75" s="20">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="H75" s="20">
-        <v>2.0000000000000001E-10</v>
+        <v>4.4999999999999998E-9</v>
       </c>
     </row>
     <row r="76" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -51674,17 +51663,17 @@
       <c r="D76" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="E76" s="47">
-        <v>4.0000000000000001E-3</v>
+      <c r="E76" s="27">
+        <v>0.09</v>
       </c>
       <c r="F76" s="26">
-        <v>3.9E-2</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="G76" s="26">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="H76" s="26">
-        <v>2.0000000000000001E-10</v>
+        <v>4.4999999999999998E-9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on presentation of results
</commit_message>
<xml_diff>
--- a/Zetas_new.xlsx
+++ b/Zetas_new.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Z541213\Documents\Project\Model\Schisto_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F0DE19-84E2-4B65-9CA2-3DAF6BD1D2BF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C026DA-222D-4FD2-80B3-163EF620C13A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -83,8 +83,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="0E+00"/>
-    <numFmt numFmtId="167" formatCode="0.0E+00"/>
+    <numFmt numFmtId="164" formatCode="0E+00"/>
+    <numFmt numFmtId="165" formatCode="0.0E+00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -264,16 +264,16 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -557,8 +557,8 @@
   <dimension ref="A1:XFC76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F34" sqref="F34"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -716,7 +716,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="6">
-        <v>1.08E-4</v>
+        <v>1.2E-4</v>
       </c>
       <c r="G6" s="6">
         <v>0.1</v>
@@ -742,7 +742,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="6">
-        <v>1.08E-4</v>
+        <v>1.2E-4</v>
       </c>
       <c r="G7" s="6">
         <v>0.1</v>
@@ -924,10 +924,10 @@
         <v>5</v>
       </c>
       <c r="E14" s="13">
-        <v>0.09</v>
+        <v>0.08</v>
       </c>
       <c r="F14" s="12">
-        <v>0.02</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="G14" s="12">
         <v>0.1</v>
@@ -950,7 +950,7 @@
         <v>6</v>
       </c>
       <c r="E15" s="13">
-        <v>0.09</v>
+        <v>0.08</v>
       </c>
       <c r="F15" s="12">
         <v>0.02</v>
@@ -976,7 +976,7 @@
         <v>7</v>
       </c>
       <c r="E16" s="13">
-        <v>0.09</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F16" s="12">
         <v>0.02</v>
@@ -1187,7 +1187,7 @@
         <v>0.09</v>
       </c>
       <c r="F24" s="18">
-        <v>3.5000000000000003E-2</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="G24" s="18">
         <v>0.1</v>
@@ -1213,7 +1213,7 @@
         <v>0.09</v>
       </c>
       <c r="F25" s="18">
-        <v>3.5000000000000003E-2</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="G25" s="18">
         <v>0.1</v>
@@ -1343,7 +1343,7 @@
         <v>0</v>
       </c>
       <c r="F30" s="4">
-        <v>1.65E-4</v>
+        <v>1.64E-4</v>
       </c>
       <c r="G30" s="4">
         <v>0.2</v>
@@ -1369,7 +1369,7 @@
         <v>0</v>
       </c>
       <c r="F31" s="4">
-        <v>1.65E-4</v>
+        <v>1.6699999999999999E-4</v>
       </c>
       <c r="G31" s="4">
         <v>0.2</v>
@@ -1499,7 +1499,7 @@
         <v>0</v>
       </c>
       <c r="F36" s="8">
-        <v>6.4999999999999997E-3</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="G36" s="8">
         <v>0.1</v>
@@ -1525,7 +1525,7 @@
         <v>0</v>
       </c>
       <c r="F37" s="8">
-        <v>6.4999999999999997E-3</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="G37" s="8">
         <v>0.1</v>
@@ -50991,7 +50991,7 @@
         <v>0.1</v>
       </c>
       <c r="F50" s="18">
-        <v>0.27</v>
+        <v>0.26</v>
       </c>
       <c r="G50" s="18">
         <v>0.2</v>

</xml_diff>

<commit_message>
Retuned moderate and low
</commit_message>
<xml_diff>
--- a/Zetas_new.xlsx
+++ b/Zetas_new.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Z541213\Documents\Project\Model\Schisto_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C026DA-222D-4FD2-80B3-163EF620C13A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D361C83B-703F-4FB0-8AEE-CBBBC53D2181}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="15">
   <si>
     <t xml:space="preserve">Endemicity </t>
   </si>
@@ -77,14 +77,18 @@
   <si>
     <t>Transmission on snails</t>
   </si>
+  <si>
+    <t>fatto</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0E+00"/>
     <numFmt numFmtId="165" formatCode="0.0E+00"/>
+    <numFmt numFmtId="170" formatCode="0.00000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -268,12 +272,12 @@
     <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="170" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -557,7 +561,7 @@
   <dimension ref="A1:XFC76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
@@ -611,11 +615,12 @@
       <c r="E2" s="3">
         <v>0</v>
       </c>
-      <c r="F2" s="2">
-        <v>8.2999999999999998E-5</v>
+      <c r="F2" s="4">
+        <f xml:space="preserve"> 0.000101*0.84</f>
+        <v>8.4839999999999994E-5</v>
       </c>
       <c r="G2" s="4">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H2" s="4">
         <v>0</v>
@@ -638,10 +643,11 @@
         <v>0</v>
       </c>
       <c r="F3" s="4">
-        <v>1.01E-4</v>
+        <f xml:space="preserve"> 0.000101*0.84</f>
+        <v>8.4839999999999994E-5</v>
       </c>
       <c r="G3" s="4">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H3" s="4">
         <v>0</v>
@@ -664,10 +670,11 @@
         <v>0</v>
       </c>
       <c r="F4" s="4">
-        <v>1.01E-4</v>
+        <f xml:space="preserve"> 0.000101*0.84</f>
+        <v>8.4839999999999994E-5</v>
       </c>
       <c r="G4" s="4">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H4" s="4">
         <v>0</v>
@@ -690,10 +697,10 @@
         <v>0</v>
       </c>
       <c r="F5" s="6">
-        <v>1.0399999999999999E-4</v>
+        <v>8.7999999999999998E-5</v>
       </c>
       <c r="G5" s="6">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H5" s="6">
         <v>0</v>
@@ -716,10 +723,10 @@
         <v>0</v>
       </c>
       <c r="F6" s="6">
-        <v>1.2E-4</v>
+        <v>8.8999999999999995E-5</v>
       </c>
       <c r="G6" s="6">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H6" s="6">
         <v>0</v>
@@ -742,10 +749,10 @@
         <v>0</v>
       </c>
       <c r="F7" s="6">
-        <v>1.2E-4</v>
+        <v>8.8999999999999995E-5</v>
       </c>
       <c r="G7" s="6">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H7" s="6">
         <v>0</v>
@@ -768,10 +775,10 @@
         <v>0</v>
       </c>
       <c r="F8" s="8">
-        <v>8.9999999999999998E-4</v>
+        <v>1.4999999999999999E-4</v>
       </c>
       <c r="G8" s="8">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
       <c r="H8" s="8">
         <v>0</v>
@@ -794,10 +801,10 @@
         <v>0</v>
       </c>
       <c r="F9" s="8">
-        <v>8.9999999999999998E-4</v>
+        <v>1.4999999999999999E-4</v>
       </c>
       <c r="G9" s="8">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
       <c r="H9" s="8">
         <v>0</v>
@@ -820,10 +827,10 @@
         <v>0</v>
       </c>
       <c r="F10" s="8">
-        <v>8.9999999999999998E-4</v>
+        <v>1.4999999999999999E-4</v>
       </c>
       <c r="G10" s="8">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
       <c r="H10" s="8">
         <v>0</v>
@@ -843,17 +850,17 @@
         <v>5</v>
       </c>
       <c r="E11" s="11">
-        <v>0.09</v>
+        <v>0.05</v>
       </c>
       <c r="F11" s="10">
-        <v>2.1999999999999999E-2</v>
+        <v>1.32E-2</v>
       </c>
       <c r="G11" s="10">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H11" s="10">
-        <f>2*10^(-10)</f>
-        <v>2.0000000000000001E-10</v>
+        <f>3*10^(-10)</f>
+        <v>3E-10</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -870,17 +877,17 @@
         <v>6</v>
       </c>
       <c r="E12" s="11">
-        <v>0.09</v>
+        <v>0.05</v>
       </c>
       <c r="F12" s="10">
-        <v>1.9E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="G12" s="10">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H12" s="10">
-        <f t="shared" ref="H12:H13" si="0">3*10^(-10)</f>
-        <v>3E-10</v>
+        <f>3.2*10^(-10)</f>
+        <v>3.2000000000000003E-10</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -897,17 +904,17 @@
         <v>7</v>
       </c>
       <c r="E13" s="11">
-        <v>0.09</v>
+        <v>0.05</v>
       </c>
       <c r="F13" s="10">
-        <v>1.9E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="G13" s="10">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H13" s="10">
-        <f t="shared" si="0"/>
-        <v>3E-10</v>
+        <f>3.2*10^(-10)</f>
+        <v>3.2000000000000003E-10</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -924,13 +931,13 @@
         <v>5</v>
       </c>
       <c r="E14" s="13">
-        <v>0.08</v>
+        <v>0.05</v>
       </c>
       <c r="F14" s="12">
-        <v>1.7999999999999999E-2</v>
+        <v>1.44E-2</v>
       </c>
       <c r="G14" s="12">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H14" s="12">
         <v>3E-10</v>
@@ -950,13 +957,13 @@
         <v>6</v>
       </c>
       <c r="E15" s="13">
-        <v>0.08</v>
+        <v>0.05</v>
       </c>
       <c r="F15" s="12">
-        <v>0.02</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="G15" s="12">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H15" s="12">
         <v>3E-10</v>
@@ -976,13 +983,13 @@
         <v>7</v>
       </c>
       <c r="E16" s="13">
-        <v>7.0000000000000007E-2</v>
+        <v>0.05</v>
       </c>
       <c r="F16" s="12">
-        <v>0.02</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="G16" s="12">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H16" s="12">
         <v>3E-10</v>
@@ -1002,16 +1009,16 @@
         <v>5</v>
       </c>
       <c r="E17" s="15">
-        <v>0.09</v>
+        <v>0.06</v>
       </c>
       <c r="F17" s="14">
-        <v>0.18</v>
+        <v>0.02</v>
       </c>
       <c r="G17" s="14">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
       <c r="H17" s="14">
-        <v>3E-10</v>
+        <v>4.0000000000000001E-10</v>
       </c>
     </row>
     <row r="18" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.3">
@@ -1028,16 +1035,16 @@
         <v>6</v>
       </c>
       <c r="E18" s="15">
-        <v>0.09</v>
+        <v>0.05</v>
       </c>
       <c r="F18" s="14">
-        <v>0.18</v>
+        <v>0.02</v>
       </c>
       <c r="G18" s="14">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
       <c r="H18" s="14">
-        <v>3E-10</v>
+        <v>4.0000000000000001E-10</v>
       </c>
     </row>
     <row r="19" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.3">
@@ -1054,16 +1061,16 @@
         <v>7</v>
       </c>
       <c r="E19" s="15">
-        <v>0.09</v>
+        <v>0.05</v>
       </c>
       <c r="F19" s="14">
-        <v>0.18</v>
+        <v>0.02</v>
       </c>
       <c r="G19" s="14">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
       <c r="H19" s="14">
-        <v>3E-10</v>
+        <v>4.0000000000000001E-10</v>
       </c>
     </row>
     <row r="20" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.3">
@@ -1080,16 +1087,16 @@
         <v>5</v>
       </c>
       <c r="E20" s="17">
-        <v>0.09</v>
+        <v>0.05</v>
       </c>
       <c r="F20" s="16">
-        <v>0.03</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="G20" s="16">
-        <v>0.1</v>
-      </c>
-      <c r="H20" s="41">
-        <v>3E-10</v>
+        <v>0.15</v>
+      </c>
+      <c r="H20" s="47">
+        <v>3.7999999999999998E-10</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.3">
@@ -1106,13 +1113,13 @@
         <v>6</v>
       </c>
       <c r="E21" s="17">
-        <v>0.09</v>
+        <v>0.06</v>
       </c>
       <c r="F21" s="16">
-        <v>2.5999999999999999E-2</v>
+        <v>2.0799999999999999E-2</v>
       </c>
       <c r="G21" s="16">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H21" s="41">
         <v>4.0000000000000001E-10</v>
@@ -1132,13 +1139,13 @@
         <v>7</v>
       </c>
       <c r="E22" s="17">
-        <v>0.09</v>
+        <v>0.06</v>
       </c>
       <c r="F22" s="16">
-        <v>2.5999999999999999E-2</v>
+        <v>2.0799999999999999E-2</v>
       </c>
       <c r="G22" s="16">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H22" s="41">
         <v>4.0000000000000001E-10</v>
@@ -1158,13 +1165,13 @@
         <v>5</v>
       </c>
       <c r="E23" s="19">
-        <v>0.09</v>
+        <v>0.05</v>
       </c>
       <c r="F23" s="18">
-        <v>3.5999999999999997E-2</v>
+        <v>2.8799999999999999E-2</v>
       </c>
       <c r="G23" s="18">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H23" s="42">
         <v>3E-10</v>
@@ -1184,13 +1191,13 @@
         <v>6</v>
       </c>
       <c r="E24" s="19">
-        <v>0.09</v>
+        <v>0.06</v>
       </c>
       <c r="F24" s="18">
-        <v>3.4000000000000002E-2</v>
+        <v>2.3E-2</v>
       </c>
       <c r="G24" s="18">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H24" s="42">
         <v>4.0000000000000001E-10</v>
@@ -1210,13 +1217,13 @@
         <v>7</v>
       </c>
       <c r="E25" s="19">
-        <v>0.09</v>
+        <v>0.06</v>
       </c>
       <c r="F25" s="18">
-        <v>3.4000000000000002E-2</v>
+        <v>2.3E-2</v>
       </c>
       <c r="G25" s="18">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H25" s="42">
         <v>4.0000000000000001E-10</v>
@@ -1236,16 +1243,16 @@
         <v>5</v>
       </c>
       <c r="E26" s="21">
-        <v>0.09</v>
+        <v>0.06</v>
       </c>
       <c r="F26" s="20">
-        <v>0.5</v>
+        <v>0.04</v>
       </c>
       <c r="G26" s="20">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
       <c r="H26" s="40">
-        <v>2.0000000000000001E-10</v>
+        <v>4.0000000000000001E-10</v>
       </c>
     </row>
     <row r="27" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.3">
@@ -1262,16 +1269,16 @@
         <v>6</v>
       </c>
       <c r="E27" s="21">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="F27" s="20">
-        <v>0.5</v>
+        <v>0.04</v>
       </c>
       <c r="G27" s="20">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
       <c r="H27" s="40">
-        <v>3E-10</v>
+        <v>4.0000000000000001E-10</v>
       </c>
     </row>
     <row r="28" spans="1:8" s="20" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1288,16 +1295,16 @@
         <v>7</v>
       </c>
       <c r="E28" s="27">
-        <v>0.08</v>
+        <v>0.05</v>
       </c>
       <c r="F28" s="26">
-        <v>0.5</v>
+        <v>0.04</v>
       </c>
       <c r="G28" s="26">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
       <c r="H28" s="43">
-        <v>3E-10</v>
+        <v>4.0000000000000001E-10</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
@@ -1317,10 +1324,11 @@
         <v>0</v>
       </c>
       <c r="F29" s="2">
-        <v>1E-4</v>
+        <f>0.0001*0.9</f>
+        <v>9.0000000000000006E-5</v>
       </c>
       <c r="G29" s="4">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="H29" s="4">
         <v>0</v>
@@ -1342,11 +1350,11 @@
       <c r="E30" s="5">
         <v>0</v>
       </c>
-      <c r="F30" s="4">
-        <v>1.64E-4</v>
+      <c r="F30" s="49">
+        <v>9.0000000000000006E-5</v>
       </c>
       <c r="G30" s="4">
-        <v>0.2</v>
+        <v>0.35</v>
       </c>
       <c r="H30" s="4">
         <v>0</v>
@@ -1369,10 +1377,10 @@
         <v>0</v>
       </c>
       <c r="F31" s="4">
-        <v>1.6699999999999999E-4</v>
+        <v>9.0000000000000006E-5</v>
       </c>
       <c r="G31" s="4">
-        <v>0.2</v>
+        <v>0.35</v>
       </c>
       <c r="H31" s="4">
         <v>0</v>
@@ -1395,10 +1403,11 @@
         <v>0</v>
       </c>
       <c r="F32" s="6">
-        <v>1.6437790000000001E-4</v>
+        <f>0.0001643779*0.9</f>
+        <v>1.4794011000000002E-4</v>
       </c>
       <c r="G32" s="6">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="H32" s="6">
         <v>0</v>
@@ -1421,10 +1430,11 @@
         <v>0</v>
       </c>
       <c r="F33" s="6">
-        <v>2.0000000000000001E-4</v>
+        <f>0.0002*0.9</f>
+        <v>1.8000000000000001E-4</v>
       </c>
       <c r="G33" s="6">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="H33" s="6">
         <v>0</v>
@@ -1447,10 +1457,11 @@
         <v>0</v>
       </c>
       <c r="F34" s="6">
-        <v>2.0000000000000001E-4</v>
+        <f>0.0002*0.9</f>
+        <v>1.8000000000000001E-4</v>
       </c>
       <c r="G34" s="6">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="H34" s="6">
         <v>0</v>
@@ -1473,10 +1484,11 @@
         <v>0</v>
       </c>
       <c r="F35" s="8">
-        <v>6.0000000000000001E-3</v>
+        <f>0.006*0.9</f>
+        <v>5.4000000000000003E-3</v>
       </c>
       <c r="G35" s="8">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="H35" s="8">
         <v>0</v>
@@ -1499,10 +1511,11 @@
         <v>0</v>
       </c>
       <c r="F36" s="8">
-        <v>7.0000000000000001E-3</v>
+        <f>0.007*0.9</f>
+        <v>6.3E-3</v>
       </c>
       <c r="G36" s="8">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="H36" s="8">
         <v>0</v>
@@ -1525,10 +1538,11 @@
         <v>0</v>
       </c>
       <c r="F37" s="8">
-        <v>7.0000000000000001E-3</v>
+        <f>0.007*0.9</f>
+        <v>6.3E-3</v>
       </c>
       <c r="G37" s="8">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="H37" s="8">
         <v>0</v>
@@ -1554,7 +1568,7 @@
         <v>0.159</v>
       </c>
       <c r="G38" s="10">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="H38" s="10">
         <f>3*10^(-11)</f>
@@ -1578,13 +1592,14 @@
         <v>0.09</v>
       </c>
       <c r="F39" s="10">
-        <v>0.158</v>
+        <f>0.158*0.9</f>
+        <v>0.14219999999999999</v>
       </c>
       <c r="G39" s="10">
-        <v>0.18</v>
+        <v>0.3</v>
       </c>
       <c r="H39" s="10">
-        <f t="shared" ref="H39:H40" si="1">7*10^(-11)</f>
+        <f t="shared" ref="H39:H40" si="0">7*10^(-11)</f>
         <v>6.9999999999999991E-11</v>
       </c>
     </row>
@@ -1605,13 +1620,14 @@
         <v>0.09</v>
       </c>
       <c r="F40" s="10">
-        <v>0.158</v>
+        <f>0.158*0.9</f>
+        <v>0.14219999999999999</v>
       </c>
       <c r="G40" s="10">
-        <v>0.18</v>
+        <v>0.3</v>
       </c>
       <c r="H40" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6.9999999999999991E-11</v>
       </c>
     </row>
@@ -1632,10 +1648,11 @@
         <v>0.09</v>
       </c>
       <c r="F41" s="12">
-        <v>0.16400000000000001</v>
+        <f>0.164*0.9</f>
+        <v>0.14760000000000001</v>
       </c>
       <c r="G41" s="12">
-        <v>0.18</v>
+        <v>0.3</v>
       </c>
       <c r="H41" s="12">
         <v>6E-11</v>
@@ -1658,10 +1675,11 @@
         <v>0.1</v>
       </c>
       <c r="F42" s="12">
-        <v>0.15</v>
+        <f>0.15*0.9</f>
+        <v>0.13500000000000001</v>
       </c>
       <c r="G42" s="12">
-        <v>0.18</v>
+        <v>0.3</v>
       </c>
       <c r="H42" s="12">
         <v>1E-10</v>
@@ -1684,10 +1702,11 @@
         <v>0.1</v>
       </c>
       <c r="F43" s="12">
-        <v>0.15</v>
+        <f>0.15*0.9</f>
+        <v>0.13500000000000001</v>
       </c>
       <c r="G43" s="12">
-        <v>0.18</v>
+        <v>0.3</v>
       </c>
       <c r="H43" s="12">
         <v>1E-10</v>
@@ -1710,10 +1729,11 @@
         <v>0.09</v>
       </c>
       <c r="F44" s="14">
-        <v>5</v>
+        <f>5*0.9</f>
+        <v>4.5</v>
       </c>
       <c r="G44" s="14">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="H44" s="14">
         <v>6E-11</v>
@@ -1736,10 +1756,11 @@
         <v>0.11</v>
       </c>
       <c r="F45" s="14">
-        <v>5</v>
+        <f t="shared" ref="F45:F46" si="1">5*0.9</f>
+        <v>4.5</v>
       </c>
       <c r="G45" s="14">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="H45" s="14">
         <v>1E-10</v>
@@ -1762,10 +1783,11 @@
         <v>0.1</v>
       </c>
       <c r="F46" s="14">
-        <v>5</v>
+        <f t="shared" si="1"/>
+        <v>4.5</v>
       </c>
       <c r="G46" s="14">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="H46" s="14">
         <v>1E-10</v>
@@ -1788,10 +1810,11 @@
         <v>0.11</v>
       </c>
       <c r="F47" s="24">
-        <v>0.15</v>
+        <f>0.15*0.9</f>
+        <v>0.13500000000000001</v>
       </c>
       <c r="G47" s="24">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="H47" s="16">
         <v>7.0000000000000004E-11</v>
@@ -18189,10 +18212,11 @@
         <v>0.09</v>
       </c>
       <c r="F48" s="24">
-        <v>0.14799999999999999</v>
+        <f>0.148*0.9</f>
+        <v>0.13319999999999999</v>
       </c>
       <c r="G48" s="24">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="H48" s="16">
         <v>1E-10</v>
@@ -34590,10 +34614,11 @@
         <v>0.09</v>
       </c>
       <c r="F49" s="24">
-        <v>0.14799999999999999</v>
+        <f>0.148*0.9</f>
+        <v>0.13319999999999999</v>
       </c>
       <c r="G49" s="24">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="H49" s="16">
         <v>1E-10</v>
@@ -50991,10 +51016,11 @@
         <v>0.1</v>
       </c>
       <c r="F50" s="18">
-        <v>0.26</v>
+        <f>0.26*0.9</f>
+        <v>0.23400000000000001</v>
       </c>
       <c r="G50" s="18">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="H50" s="18">
         <v>7.0000000000000004E-11</v>
@@ -51014,16 +51040,19 @@
         <v>6</v>
       </c>
       <c r="E51" s="19">
-        <v>0.1</v>
+        <v>0.06</v>
       </c>
       <c r="F51" s="18">
-        <v>0.55000000000000004</v>
+        <v>0.13</v>
       </c>
       <c r="G51" s="18">
-        <v>0.15</v>
+        <v>0.3</v>
       </c>
       <c r="H51" s="18">
         <v>8.9999999999999999E-11</v>
+      </c>
+      <c r="I51" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="52" spans="1:16383" x14ac:dyDescent="0.3">
@@ -51040,16 +51069,19 @@
         <v>7</v>
       </c>
       <c r="E52" s="19">
-        <v>0.1</v>
+        <v>0.06</v>
       </c>
       <c r="F52" s="18">
-        <v>0.55000000000000004</v>
+        <v>0.13</v>
       </c>
       <c r="G52" s="18">
-        <v>0.15</v>
+        <v>0.3</v>
       </c>
       <c r="H52" s="18">
         <v>8.9999999999999999E-11</v>
+      </c>
+      <c r="I52" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="53" spans="1:16383" x14ac:dyDescent="0.3">
@@ -51069,10 +51101,11 @@
         <v>0.11</v>
       </c>
       <c r="F53" s="20">
-        <v>9</v>
+        <f>9*0.9</f>
+        <v>8.1</v>
       </c>
       <c r="G53" s="20">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="H53" s="40">
         <v>7.0000000000000004E-11</v>
@@ -51095,10 +51128,11 @@
         <v>0.1</v>
       </c>
       <c r="F54" s="20">
-        <v>8</v>
+        <f>8*0.9</f>
+        <v>7.2</v>
       </c>
       <c r="G54" s="20">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="H54" s="40">
         <v>1E-10</v>
@@ -51121,10 +51155,11 @@
         <v>0.1</v>
       </c>
       <c r="F55" s="26">
-        <v>8</v>
+        <f>8*0.9</f>
+        <v>7.2</v>
       </c>
       <c r="G55" s="26">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="H55" s="43">
         <v>1E-10</v>
@@ -51147,7 +51182,7 @@
         <v>0</v>
       </c>
       <c r="F56" s="8">
-        <v>8.7999999999999998E-5</v>
+        <v>9.0000000000000006E-5</v>
       </c>
       <c r="G56" s="8">
         <v>0.1</v>
@@ -51222,16 +51257,17 @@
         <v>5</v>
       </c>
       <c r="E59" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="F59" s="10">
+        <v>9.7999999999999997E-4</v>
+      </c>
+      <c r="G59" s="10">
         <v>0.1</v>
       </c>
-      <c r="F59" s="10">
-        <v>8.9999999999999998E-4</v>
-      </c>
-      <c r="G59" s="10">
-        <v>0.05</v>
-      </c>
       <c r="H59" s="44">
-        <v>4.8E-9</v>
+        <f>0.000000004</f>
+        <v>4.0000000000000002E-9</v>
       </c>
     </row>
     <row r="60" spans="1:16383" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -51248,16 +51284,17 @@
         <v>6</v>
       </c>
       <c r="E60" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="F60" s="10">
+        <v>9.7999999999999997E-4</v>
+      </c>
+      <c r="G60" s="10">
         <v>0.1</v>
       </c>
-      <c r="F60" s="10">
-        <v>8.9999999999999998E-4</v>
-      </c>
-      <c r="G60" s="10">
-        <v>0.05</v>
-      </c>
-      <c r="H60" s="45">
-        <v>5.0000000000000001E-9</v>
+      <c r="H60" s="44">
+        <f>0.000000005*0.8</f>
+        <v>4.0000000000000002E-9</v>
       </c>
     </row>
     <row r="61" spans="1:16383" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -51274,16 +51311,17 @@
         <v>7</v>
       </c>
       <c r="E61" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="F61" s="10">
+        <v>9.7999999999999997E-4</v>
+      </c>
+      <c r="G61" s="10">
         <v>0.1</v>
       </c>
-      <c r="F61" s="10">
-        <v>8.9999999999999998E-4</v>
-      </c>
-      <c r="G61" s="10">
-        <v>0.05</v>
-      </c>
-      <c r="H61" s="45">
-        <v>5.0000000000000001E-9</v>
+      <c r="H61" s="44">
+        <f>0.000000005*0.8</f>
+        <v>4.0000000000000002E-9</v>
       </c>
     </row>
     <row r="62" spans="1:16383" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -51300,16 +51338,16 @@
         <v>5</v>
       </c>
       <c r="E62" s="13">
+        <v>0.06</v>
+      </c>
+      <c r="F62" s="12">
+        <v>9.8999999999999999E-4</v>
+      </c>
+      <c r="G62" s="12">
         <v>0.1</v>
       </c>
-      <c r="F62" s="12">
-        <v>8.9999999999999998E-4</v>
-      </c>
-      <c r="G62" s="12">
-        <v>0.05</v>
-      </c>
-      <c r="H62" s="46">
-        <v>5.0000000000000001E-9</v>
+      <c r="H62" s="45">
+        <v>4.0000000000000002E-9</v>
       </c>
     </row>
     <row r="63" spans="1:16383" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -51326,16 +51364,16 @@
         <v>6</v>
       </c>
       <c r="E63" s="13">
+        <v>0.06</v>
+      </c>
+      <c r="F63" s="12">
+        <v>9.8999999999999999E-4</v>
+      </c>
+      <c r="G63" s="12">
         <v>0.1</v>
       </c>
-      <c r="F63" s="12">
-        <v>8.9999999999999998E-4</v>
-      </c>
-      <c r="G63" s="12">
-        <v>0.05</v>
-      </c>
-      <c r="H63" s="46">
-        <v>5.0000000000000001E-9</v>
+      <c r="H63" s="45">
+        <v>4.0000000000000002E-9</v>
       </c>
     </row>
     <row r="64" spans="1:16383" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -51352,16 +51390,16 @@
         <v>7</v>
       </c>
       <c r="E64" s="13">
-        <v>0.09</v>
+        <v>0.06</v>
       </c>
       <c r="F64" s="12">
-        <v>8.9999999999999998E-4</v>
+        <v>9.8999999999999999E-4</v>
       </c>
       <c r="G64" s="12">
-        <v>0.05</v>
-      </c>
-      <c r="H64" s="46">
-        <v>5.0000000000000001E-9</v>
+        <v>0.1</v>
+      </c>
+      <c r="H64" s="45">
+        <v>4.0000000000000002E-9</v>
       </c>
     </row>
     <row r="65" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.3">
@@ -51378,16 +51416,17 @@
         <v>5</v>
       </c>
       <c r="E65" s="15">
-        <v>0.09</v>
+        <v>0.06</v>
       </c>
       <c r="F65" s="14">
-        <v>1.1000000000000001E-3</v>
+        <f>0.00121*0.9</f>
+        <v>1.0889999999999999E-3</v>
       </c>
       <c r="G65" s="14">
-        <v>0.05</v>
-      </c>
-      <c r="H65" s="47">
-        <v>5.0000000000000001E-9</v>
+        <v>0.1</v>
+      </c>
+      <c r="H65" s="46">
+        <v>4.0000000000000002E-9</v>
       </c>
     </row>
     <row r="66" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.3">
@@ -51404,16 +51443,17 @@
         <v>6</v>
       </c>
       <c r="E66" s="15">
-        <v>0.09</v>
+        <v>0.06</v>
       </c>
       <c r="F66" s="14">
-        <v>1.1000000000000001E-3</v>
+        <f t="shared" ref="F66:F67" si="2">0.00121*0.9</f>
+        <v>1.0889999999999999E-3</v>
       </c>
       <c r="G66" s="14">
-        <v>0.05</v>
-      </c>
-      <c r="H66" s="47">
-        <v>5.0000000000000001E-9</v>
+        <v>0.1</v>
+      </c>
+      <c r="H66" s="46">
+        <v>4.0000000000000002E-9</v>
       </c>
     </row>
     <row r="67" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.3">
@@ -51430,16 +51470,17 @@
         <v>7</v>
       </c>
       <c r="E67" s="15">
-        <v>0.09</v>
+        <v>0.06</v>
       </c>
       <c r="F67" s="14">
-        <v>1.1000000000000001E-3</v>
+        <f t="shared" si="2"/>
+        <v>1.0889999999999999E-3</v>
       </c>
       <c r="G67" s="14">
-        <v>0.05</v>
-      </c>
-      <c r="H67" s="47">
-        <v>5.0000000000000001E-9</v>
+        <v>0.1</v>
+      </c>
+      <c r="H67" s="46">
+        <v>4.0000000000000002E-9</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
@@ -51456,16 +51497,17 @@
         <v>5</v>
       </c>
       <c r="E68" s="25">
+        <v>0.06</v>
+      </c>
+      <c r="F68" s="24">
+        <v>2.2000000000000001E-3</v>
+      </c>
+      <c r="G68" s="24">
         <v>0.1</v>
       </c>
-      <c r="F68" s="24">
-        <v>2E-3</v>
-      </c>
-      <c r="G68" s="24">
-        <v>0.05</v>
-      </c>
-      <c r="H68" s="48">
-        <v>4.4999999999999998E-9</v>
+      <c r="H68" s="47">
+        <f>0.0000000045*0.8</f>
+        <v>3.6E-9</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.3">
@@ -51482,16 +51524,17 @@
         <v>6</v>
       </c>
       <c r="E69" s="25">
+        <v>0.06</v>
+      </c>
+      <c r="F69" s="24">
+        <v>2.2000000000000001E-3</v>
+      </c>
+      <c r="G69" s="24">
         <v>0.1</v>
       </c>
-      <c r="F69" s="24">
-        <v>2E-3</v>
-      </c>
-      <c r="G69" s="24">
-        <v>0.05</v>
-      </c>
-      <c r="H69" s="48">
-        <v>4.4999999999999998E-9</v>
+      <c r="H69" s="47">
+        <f t="shared" ref="H69:H70" si="3">0.0000000045*0.8</f>
+        <v>3.6E-9</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
@@ -51508,16 +51551,17 @@
         <v>7</v>
       </c>
       <c r="E70" s="25">
+        <v>0.06</v>
+      </c>
+      <c r="F70" s="24">
+        <v>2.2000000000000001E-3</v>
+      </c>
+      <c r="G70" s="24">
         <v>0.1</v>
       </c>
-      <c r="F70" s="24">
-        <v>2E-3</v>
-      </c>
-      <c r="G70" s="24">
-        <v>0.05</v>
-      </c>
-      <c r="H70" s="48">
-        <v>4.4999999999999998E-9</v>
+      <c r="H70" s="47">
+        <f t="shared" si="3"/>
+        <v>3.6E-9</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.3">
@@ -51534,16 +51578,16 @@
         <v>5</v>
       </c>
       <c r="E71" s="19">
-        <v>0.09</v>
+        <v>0.06</v>
       </c>
       <c r="F71" s="18">
-        <v>2E-3</v>
+        <v>2.2000000000000001E-3</v>
       </c>
       <c r="G71" s="18">
-        <v>0.05</v>
-      </c>
-      <c r="H71" s="49">
-        <v>4.4999999999999998E-9</v>
+        <v>0.1</v>
+      </c>
+      <c r="H71" s="48">
+        <v>3.6E-9</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.3">
@@ -51560,16 +51604,16 @@
         <v>6</v>
       </c>
       <c r="E72" s="19">
-        <v>0.09</v>
+        <v>0.06</v>
       </c>
       <c r="F72" s="18">
-        <v>2E-3</v>
+        <v>2.2000000000000001E-3</v>
       </c>
       <c r="G72" s="18">
-        <v>0.05</v>
-      </c>
-      <c r="H72" s="49">
-        <v>4.4999999999999998E-9</v>
+        <v>0.1</v>
+      </c>
+      <c r="H72" s="48">
+        <v>3.6E-9</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.3">
@@ -51586,16 +51630,16 @@
         <v>7</v>
       </c>
       <c r="E73" s="19">
-        <v>0.09</v>
+        <v>0.06</v>
       </c>
       <c r="F73" s="18">
-        <v>2E-3</v>
+        <v>2.2000000000000001E-3</v>
       </c>
       <c r="G73" s="18">
-        <v>0.05</v>
-      </c>
-      <c r="H73" s="49">
-        <v>4.4999999999999998E-9</v>
+        <v>0.1</v>
+      </c>
+      <c r="H73" s="48">
+        <v>3.6E-9</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.3">
@@ -51612,16 +51656,17 @@
         <v>5</v>
       </c>
       <c r="E74" s="21">
-        <v>0.09</v>
+        <v>0.06</v>
       </c>
       <c r="F74" s="20">
-        <v>2.5000000000000001E-3</v>
+        <f>0.00275*0.9</f>
+        <v>2.4749999999999998E-3</v>
       </c>
       <c r="G74" s="20">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="H74" s="20">
-        <v>4.4999999999999998E-9</v>
+        <v>3.6E-9</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.3">
@@ -51638,16 +51683,17 @@
         <v>6</v>
       </c>
       <c r="E75" s="21">
-        <v>0.09</v>
+        <v>0.06</v>
       </c>
       <c r="F75" s="20">
-        <v>2.5000000000000001E-3</v>
+        <f t="shared" ref="F75:F76" si="4">0.00275*0.9</f>
+        <v>2.4749999999999998E-3</v>
       </c>
       <c r="G75" s="20">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="H75" s="20">
-        <v>4.4999999999999998E-9</v>
+        <v>3.6E-9</v>
       </c>
     </row>
     <row r="76" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -51664,16 +51710,17 @@
         <v>7</v>
       </c>
       <c r="E76" s="27">
-        <v>0.09</v>
+        <v>0.06</v>
       </c>
       <c r="F76" s="26">
-        <v>2.5000000000000001E-3</v>
+        <f t="shared" si="4"/>
+        <v>2.4749999999999998E-3</v>
       </c>
       <c r="G76" s="26">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="H76" s="26">
-        <v>4.4999999999999998E-9</v>
+        <v>3.6E-9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Code adapted to allow a user-defined exposure function
</commit_message>
<xml_diff>
--- a/Zetas_new.xlsx
+++ b/Zetas_new.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Z541213\Documents\Project\Model\Schisto_model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Z541213\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D361C83B-703F-4FB0-8AEE-CBBBC53D2181}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0453869-CA0A-4A69-B6D6-E647EBB001E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="14">
   <si>
     <t xml:space="preserve">Endemicity </t>
   </si>
@@ -77,9 +77,6 @@
   <si>
     <t>Transmission on snails</t>
   </si>
-  <si>
-    <t>fatto</t>
-  </si>
 </sst>
 </file>
 
@@ -88,7 +85,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0E+00"/>
     <numFmt numFmtId="165" formatCode="0.0E+00"/>
-    <numFmt numFmtId="170" formatCode="0.00000"/>
+    <numFmt numFmtId="168" formatCode="0.000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -227,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -277,7 +274,9 @@
     <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="170" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -561,8 +560,8 @@
   <dimension ref="A1:XFC76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S18" sqref="S18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -573,7 +572,7 @@
     <col min="8" max="8" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -599,7 +598,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="28" t="s">
         <v>4</v>
       </c>
@@ -615,18 +614,23 @@
       <c r="E2" s="3">
         <v>0</v>
       </c>
-      <c r="F2" s="4">
-        <f xml:space="preserve"> 0.000101*0.84</f>
-        <v>8.4839999999999994E-5</v>
-      </c>
-      <c r="G2" s="4">
-        <v>0.15</v>
-      </c>
-      <c r="H2" s="4">
-        <v>0</v>
-      </c>
+      <c r="I2"/>
+      <c r="J2"/>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2"/>
+      <c r="N2"/>
+      <c r="O2"/>
+      <c r="P2"/>
+      <c r="Q2"/>
+      <c r="R2"/>
+      <c r="S2"/>
+      <c r="T2"/>
+      <c r="U2"/>
+      <c r="V2"/>
+      <c r="W2"/>
     </row>
-    <row r="3" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
         <v>4</v>
       </c>
@@ -652,8 +656,23 @@
       <c r="H3" s="4">
         <v>0</v>
       </c>
+      <c r="I3"/>
+      <c r="J3"/>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
+      <c r="N3"/>
+      <c r="O3"/>
+      <c r="P3"/>
+      <c r="Q3"/>
+      <c r="R3"/>
+      <c r="S3"/>
+      <c r="T3"/>
+      <c r="U3"/>
+      <c r="V3"/>
+      <c r="W3"/>
     </row>
-    <row r="4" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
         <v>4</v>
       </c>
@@ -679,8 +698,23 @@
       <c r="H4" s="4">
         <v>0</v>
       </c>
+      <c r="I4"/>
+      <c r="J4"/>
+      <c r="K4"/>
+      <c r="L4"/>
+      <c r="M4"/>
+      <c r="N4"/>
+      <c r="O4"/>
+      <c r="P4"/>
+      <c r="Q4"/>
+      <c r="R4"/>
+      <c r="S4"/>
+      <c r="T4"/>
+      <c r="U4"/>
+      <c r="V4"/>
+      <c r="W4"/>
     </row>
-    <row r="5" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="30" t="s">
         <v>4</v>
       </c>
@@ -705,8 +739,23 @@
       <c r="H5" s="6">
         <v>0</v>
       </c>
+      <c r="I5"/>
+      <c r="J5"/>
+      <c r="K5"/>
+      <c r="L5"/>
+      <c r="M5"/>
+      <c r="N5"/>
+      <c r="O5"/>
+      <c r="P5"/>
+      <c r="Q5"/>
+      <c r="R5"/>
+      <c r="S5"/>
+      <c r="T5"/>
+      <c r="U5"/>
+      <c r="V5"/>
+      <c r="W5"/>
     </row>
-    <row r="6" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="30" t="s">
         <v>4</v>
       </c>
@@ -731,8 +780,23 @@
       <c r="H6" s="6">
         <v>0</v>
       </c>
+      <c r="I6"/>
+      <c r="J6"/>
+      <c r="K6"/>
+      <c r="L6"/>
+      <c r="M6"/>
+      <c r="N6"/>
+      <c r="O6"/>
+      <c r="P6"/>
+      <c r="Q6"/>
+      <c r="R6"/>
+      <c r="S6"/>
+      <c r="T6"/>
+      <c r="U6"/>
+      <c r="V6"/>
+      <c r="W6"/>
     </row>
-    <row r="7" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="30" t="s">
         <v>4</v>
       </c>
@@ -757,8 +821,23 @@
       <c r="H7" s="6">
         <v>0</v>
       </c>
+      <c r="I7"/>
+      <c r="J7"/>
+      <c r="K7"/>
+      <c r="L7"/>
+      <c r="M7"/>
+      <c r="N7"/>
+      <c r="O7"/>
+      <c r="P7"/>
+      <c r="Q7"/>
+      <c r="R7"/>
+      <c r="S7"/>
+      <c r="T7"/>
+      <c r="U7"/>
+      <c r="V7"/>
+      <c r="W7"/>
     </row>
-    <row r="8" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="31" t="s">
         <v>4</v>
       </c>
@@ -783,8 +862,23 @@
       <c r="H8" s="8">
         <v>0</v>
       </c>
+      <c r="I8"/>
+      <c r="J8"/>
+      <c r="K8"/>
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="N8"/>
+      <c r="O8"/>
+      <c r="P8"/>
+      <c r="Q8"/>
+      <c r="R8"/>
+      <c r="S8"/>
+      <c r="T8"/>
+      <c r="U8"/>
+      <c r="V8"/>
+      <c r="W8"/>
     </row>
-    <row r="9" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="31" t="s">
         <v>4</v>
       </c>
@@ -809,8 +903,23 @@
       <c r="H9" s="8">
         <v>0</v>
       </c>
+      <c r="I9"/>
+      <c r="J9"/>
+      <c r="K9"/>
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
+      <c r="O9"/>
+      <c r="P9"/>
+      <c r="Q9"/>
+      <c r="R9"/>
+      <c r="S9"/>
+      <c r="T9"/>
+      <c r="U9"/>
+      <c r="V9"/>
+      <c r="W9"/>
     </row>
-    <row r="10" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="31" t="s">
         <v>4</v>
       </c>
@@ -835,8 +944,23 @@
       <c r="H10" s="8">
         <v>0</v>
       </c>
+      <c r="I10"/>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10"/>
+      <c r="P10"/>
+      <c r="Q10"/>
+      <c r="R10"/>
+      <c r="S10"/>
+      <c r="T10"/>
+      <c r="U10"/>
+      <c r="V10"/>
+      <c r="W10"/>
     </row>
-    <row r="11" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="36" t="s">
         <v>4</v>
       </c>
@@ -862,8 +986,23 @@
         <f>3*10^(-10)</f>
         <v>3E-10</v>
       </c>
+      <c r="I11"/>
+      <c r="J11"/>
+      <c r="K11"/>
+      <c r="L11"/>
+      <c r="M11"/>
+      <c r="N11"/>
+      <c r="O11"/>
+      <c r="P11"/>
+      <c r="Q11"/>
+      <c r="R11"/>
+      <c r="S11"/>
+      <c r="T11"/>
+      <c r="U11"/>
+      <c r="V11"/>
+      <c r="W11"/>
     </row>
-    <row r="12" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="36" t="s">
         <v>4</v>
       </c>
@@ -889,8 +1028,23 @@
         <f>3.2*10^(-10)</f>
         <v>3.2000000000000003E-10</v>
       </c>
+      <c r="I12"/>
+      <c r="J12"/>
+      <c r="K12"/>
+      <c r="L12"/>
+      <c r="M12"/>
+      <c r="N12"/>
+      <c r="O12"/>
+      <c r="P12"/>
+      <c r="Q12"/>
+      <c r="R12"/>
+      <c r="S12"/>
+      <c r="T12"/>
+      <c r="U12"/>
+      <c r="V12"/>
+      <c r="W12"/>
     </row>
-    <row r="13" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="36" t="s">
         <v>4</v>
       </c>
@@ -916,8 +1070,23 @@
         <f>3.2*10^(-10)</f>
         <v>3.2000000000000003E-10</v>
       </c>
+      <c r="I13"/>
+      <c r="J13"/>
+      <c r="K13"/>
+      <c r="L13"/>
+      <c r="M13"/>
+      <c r="N13"/>
+      <c r="O13"/>
+      <c r="P13"/>
+      <c r="Q13"/>
+      <c r="R13"/>
+      <c r="S13"/>
+      <c r="T13"/>
+      <c r="U13"/>
+      <c r="V13"/>
+      <c r="W13"/>
     </row>
-    <row r="14" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="37" t="s">
         <v>4</v>
       </c>
@@ -942,8 +1111,23 @@
       <c r="H14" s="12">
         <v>3E-10</v>
       </c>
+      <c r="I14"/>
+      <c r="J14"/>
+      <c r="K14"/>
+      <c r="L14"/>
+      <c r="M14"/>
+      <c r="N14"/>
+      <c r="O14"/>
+      <c r="P14"/>
+      <c r="Q14"/>
+      <c r="R14"/>
+      <c r="S14"/>
+      <c r="T14"/>
+      <c r="U14"/>
+      <c r="V14"/>
+      <c r="W14"/>
     </row>
-    <row r="15" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="37" t="s">
         <v>4</v>
       </c>
@@ -968,8 +1152,23 @@
       <c r="H15" s="12">
         <v>3E-10</v>
       </c>
+      <c r="I15"/>
+      <c r="J15"/>
+      <c r="K15"/>
+      <c r="L15"/>
+      <c r="M15"/>
+      <c r="N15"/>
+      <c r="O15"/>
+      <c r="P15"/>
+      <c r="Q15"/>
+      <c r="R15"/>
+      <c r="S15"/>
+      <c r="T15"/>
+      <c r="U15"/>
+      <c r="V15"/>
+      <c r="W15"/>
     </row>
-    <row r="16" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="37" t="s">
         <v>4</v>
       </c>
@@ -994,8 +1193,23 @@
       <c r="H16" s="12">
         <v>3E-10</v>
       </c>
+      <c r="I16"/>
+      <c r="J16"/>
+      <c r="K16"/>
+      <c r="L16"/>
+      <c r="M16"/>
+      <c r="N16"/>
+      <c r="O16"/>
+      <c r="P16"/>
+      <c r="Q16"/>
+      <c r="R16"/>
+      <c r="S16"/>
+      <c r="T16"/>
+      <c r="U16"/>
+      <c r="V16"/>
+      <c r="W16"/>
     </row>
-    <row r="17" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="38" t="s">
         <v>4</v>
       </c>
@@ -1020,8 +1234,23 @@
       <c r="H17" s="14">
         <v>4.0000000000000001E-10</v>
       </c>
+      <c r="I17"/>
+      <c r="J17"/>
+      <c r="K17"/>
+      <c r="L17"/>
+      <c r="M17"/>
+      <c r="N17"/>
+      <c r="O17"/>
+      <c r="P17"/>
+      <c r="Q17"/>
+      <c r="R17"/>
+      <c r="S17"/>
+      <c r="T17"/>
+      <c r="U17"/>
+      <c r="V17"/>
+      <c r="W17"/>
     </row>
-    <row r="18" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="38" t="s">
         <v>4</v>
       </c>
@@ -1046,8 +1275,23 @@
       <c r="H18" s="14">
         <v>4.0000000000000001E-10</v>
       </c>
+      <c r="I18"/>
+      <c r="J18"/>
+      <c r="K18"/>
+      <c r="L18"/>
+      <c r="M18"/>
+      <c r="N18"/>
+      <c r="O18"/>
+      <c r="P18"/>
+      <c r="Q18"/>
+      <c r="R18"/>
+      <c r="S18"/>
+      <c r="T18"/>
+      <c r="U18"/>
+      <c r="V18"/>
+      <c r="W18"/>
     </row>
-    <row r="19" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:23" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="38" t="s">
         <v>4</v>
       </c>
@@ -1072,8 +1316,23 @@
       <c r="H19" s="14">
         <v>4.0000000000000001E-10</v>
       </c>
+      <c r="I19"/>
+      <c r="J19"/>
+      <c r="K19"/>
+      <c r="L19"/>
+      <c r="M19"/>
+      <c r="N19"/>
+      <c r="O19"/>
+      <c r="P19"/>
+      <c r="Q19"/>
+      <c r="R19"/>
+      <c r="S19"/>
+      <c r="T19"/>
+      <c r="U19"/>
+      <c r="V19"/>
+      <c r="W19"/>
     </row>
-    <row r="20" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:23" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="32" t="s">
         <v>4</v>
       </c>
@@ -1098,8 +1357,23 @@
       <c r="H20" s="47">
         <v>3.7999999999999998E-10</v>
       </c>
+      <c r="I20"/>
+      <c r="J20"/>
+      <c r="K20"/>
+      <c r="L20"/>
+      <c r="M20"/>
+      <c r="N20"/>
+      <c r="O20"/>
+      <c r="P20"/>
+      <c r="Q20"/>
+      <c r="R20"/>
+      <c r="S20"/>
+      <c r="T20"/>
+      <c r="U20"/>
+      <c r="V20"/>
+      <c r="W20"/>
     </row>
-    <row r="21" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:23" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="32" t="s">
         <v>4</v>
       </c>
@@ -1124,8 +1398,23 @@
       <c r="H21" s="41">
         <v>4.0000000000000001E-10</v>
       </c>
+      <c r="I21"/>
+      <c r="J21"/>
+      <c r="K21"/>
+      <c r="L21"/>
+      <c r="M21"/>
+      <c r="N21"/>
+      <c r="O21"/>
+      <c r="P21"/>
+      <c r="Q21"/>
+      <c r="R21"/>
+      <c r="S21"/>
+      <c r="T21"/>
+      <c r="U21"/>
+      <c r="V21"/>
+      <c r="W21"/>
     </row>
-    <row r="22" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:23" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="32" t="s">
         <v>4</v>
       </c>
@@ -1150,8 +1439,23 @@
       <c r="H22" s="41">
         <v>4.0000000000000001E-10</v>
       </c>
+      <c r="I22"/>
+      <c r="J22"/>
+      <c r="K22"/>
+      <c r="L22"/>
+      <c r="M22"/>
+      <c r="N22"/>
+      <c r="O22"/>
+      <c r="P22"/>
+      <c r="Q22"/>
+      <c r="R22"/>
+      <c r="S22"/>
+      <c r="T22"/>
+      <c r="U22"/>
+      <c r="V22"/>
+      <c r="W22"/>
     </row>
-    <row r="23" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:23" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="33" t="s">
         <v>4</v>
       </c>
@@ -1176,8 +1480,23 @@
       <c r="H23" s="42">
         <v>3E-10</v>
       </c>
+      <c r="I23"/>
+      <c r="J23"/>
+      <c r="K23"/>
+      <c r="L23"/>
+      <c r="M23"/>
+      <c r="N23"/>
+      <c r="O23"/>
+      <c r="P23"/>
+      <c r="Q23"/>
+      <c r="R23"/>
+      <c r="S23"/>
+      <c r="T23"/>
+      <c r="U23"/>
+      <c r="V23"/>
+      <c r="W23"/>
     </row>
-    <row r="24" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:23" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="33" t="s">
         <v>4</v>
       </c>
@@ -1202,8 +1521,23 @@
       <c r="H24" s="42">
         <v>4.0000000000000001E-10</v>
       </c>
+      <c r="I24"/>
+      <c r="J24"/>
+      <c r="K24"/>
+      <c r="L24"/>
+      <c r="M24"/>
+      <c r="N24"/>
+      <c r="O24"/>
+      <c r="P24"/>
+      <c r="Q24"/>
+      <c r="R24"/>
+      <c r="S24"/>
+      <c r="T24"/>
+      <c r="U24"/>
+      <c r="V24"/>
+      <c r="W24"/>
     </row>
-    <row r="25" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:23" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="33" t="s">
         <v>4</v>
       </c>
@@ -1228,8 +1562,23 @@
       <c r="H25" s="42">
         <v>4.0000000000000001E-10</v>
       </c>
+      <c r="I25"/>
+      <c r="J25"/>
+      <c r="K25"/>
+      <c r="L25"/>
+      <c r="M25"/>
+      <c r="N25"/>
+      <c r="O25"/>
+      <c r="P25"/>
+      <c r="Q25"/>
+      <c r="R25"/>
+      <c r="S25"/>
+      <c r="T25"/>
+      <c r="U25"/>
+      <c r="V25"/>
+      <c r="W25"/>
     </row>
-    <row r="26" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="34" t="s">
         <v>4</v>
       </c>
@@ -1254,8 +1603,23 @@
       <c r="H26" s="40">
         <v>4.0000000000000001E-10</v>
       </c>
+      <c r="I26"/>
+      <c r="J26"/>
+      <c r="K26"/>
+      <c r="L26"/>
+      <c r="M26"/>
+      <c r="N26"/>
+      <c r="O26"/>
+      <c r="P26"/>
+      <c r="Q26"/>
+      <c r="R26"/>
+      <c r="S26"/>
+      <c r="T26"/>
+      <c r="U26"/>
+      <c r="V26"/>
+      <c r="W26"/>
     </row>
-    <row r="27" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="34" t="s">
         <v>4</v>
       </c>
@@ -1280,8 +1644,23 @@
       <c r="H27" s="40">
         <v>4.0000000000000001E-10</v>
       </c>
+      <c r="I27"/>
+      <c r="J27"/>
+      <c r="K27"/>
+      <c r="L27"/>
+      <c r="M27"/>
+      <c r="N27"/>
+      <c r="O27"/>
+      <c r="P27"/>
+      <c r="Q27"/>
+      <c r="R27"/>
+      <c r="S27"/>
+      <c r="T27"/>
+      <c r="U27"/>
+      <c r="V27"/>
+      <c r="W27"/>
     </row>
-    <row r="28" spans="1:8" s="20" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:23" s="20" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="35" t="s">
         <v>4</v>
       </c>
@@ -1306,8 +1685,23 @@
       <c r="H28" s="43">
         <v>4.0000000000000001E-10</v>
       </c>
+      <c r="I28"/>
+      <c r="J28"/>
+      <c r="K28"/>
+      <c r="L28"/>
+      <c r="M28"/>
+      <c r="N28"/>
+      <c r="O28"/>
+      <c r="P28"/>
+      <c r="Q28"/>
+      <c r="R28"/>
+      <c r="S28"/>
+      <c r="T28"/>
+      <c r="U28"/>
+      <c r="V28"/>
+      <c r="W28"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A29" s="28" t="s">
         <v>11</v>
       </c>
@@ -1323,18 +1717,11 @@
       <c r="E29" s="3">
         <v>0</v>
       </c>
-      <c r="F29" s="2">
-        <f>0.0001*0.9</f>
-        <v>9.0000000000000006E-5</v>
-      </c>
-      <c r="G29" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="H29" s="4">
-        <v>0</v>
-      </c>
+      <c r="F29" s="2"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A30" s="29" t="s">
         <v>11</v>
       </c>
@@ -1351,7 +1738,7 @@
         <v>0</v>
       </c>
       <c r="F30" s="49">
-        <v>9.0000000000000006E-5</v>
+        <v>9.5000000000000005E-5</v>
       </c>
       <c r="G30" s="4">
         <v>0.35</v>
@@ -1360,7 +1747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A31" s="29" t="s">
         <v>11</v>
       </c>
@@ -1377,7 +1764,7 @@
         <v>0</v>
       </c>
       <c r="F31" s="4">
-        <v>9.0000000000000006E-5</v>
+        <v>9.3999999999999994E-5</v>
       </c>
       <c r="G31" s="4">
         <v>0.35</v>
@@ -1386,7 +1773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A32" s="30" t="s">
         <v>11</v>
       </c>
@@ -1403,8 +1790,8 @@
         <v>0</v>
       </c>
       <c r="F32" s="6">
-        <f>0.0001643779*0.9</f>
-        <v>1.4794011000000002E-4</v>
+        <f>0.000115</f>
+        <v>1.15E-4</v>
       </c>
       <c r="G32" s="6">
         <v>0.3</v>
@@ -1430,8 +1817,8 @@
         <v>0</v>
       </c>
       <c r="F33" s="6">
-        <f>0.0002*0.9</f>
-        <v>1.8000000000000001E-4</v>
+        <f>0.000112</f>
+        <v>1.12E-4</v>
       </c>
       <c r="G33" s="6">
         <v>0.3</v>
@@ -1457,8 +1844,8 @@
         <v>0</v>
       </c>
       <c r="F34" s="6">
-        <f>0.0002*0.9</f>
-        <v>1.8000000000000001E-4</v>
+        <f>0.000112</f>
+        <v>1.12E-4</v>
       </c>
       <c r="G34" s="6">
         <v>0.3</v>
@@ -1484,8 +1871,8 @@
         <v>0</v>
       </c>
       <c r="F35" s="8">
-        <f>0.006*0.9</f>
-        <v>5.4000000000000003E-3</v>
+        <f>0.00026</f>
+        <v>2.5999999999999998E-4</v>
       </c>
       <c r="G35" s="8">
         <v>0.25</v>
@@ -1511,8 +1898,8 @@
         <v>0</v>
       </c>
       <c r="F36" s="8">
-        <f>0.007*0.9</f>
-        <v>6.3E-3</v>
+        <f>0.00025</f>
+        <v>2.5000000000000001E-4</v>
       </c>
       <c r="G36" s="8">
         <v>0.25</v>
@@ -1538,8 +1925,8 @@
         <v>0</v>
       </c>
       <c r="F37" s="8">
-        <f>0.007*0.9</f>
-        <v>6.3E-3</v>
+        <f>0.00025</f>
+        <v>2.5000000000000001E-4</v>
       </c>
       <c r="G37" s="8">
         <v>0.25</v>
@@ -1562,18 +1949,31 @@
         <v>5</v>
       </c>
       <c r="E38" s="11">
-        <v>0.08</v>
+        <v>0.06</v>
       </c>
       <c r="F38" s="10">
-        <v>0.159</v>
+        <v>5.33E-2</v>
       </c>
       <c r="G38" s="10">
         <v>0.3</v>
       </c>
       <c r="H38" s="10">
-        <f>3*10^(-11)</f>
-        <v>3E-11</v>
-      </c>
+        <f>9*10^(-11)</f>
+        <v>8.9999999999999999E-11</v>
+      </c>
+      <c r="I38"/>
+      <c r="J38"/>
+      <c r="K38"/>
+      <c r="L38"/>
+      <c r="M38"/>
+      <c r="N38"/>
+      <c r="O38"/>
+      <c r="P38"/>
+      <c r="Q38"/>
+      <c r="R38"/>
+      <c r="S38"/>
+      <c r="T38"/>
+      <c r="U38"/>
     </row>
     <row r="39" spans="1:16383" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="36" t="s">
@@ -1589,19 +1989,31 @@
         <v>6</v>
       </c>
       <c r="E39" s="11">
-        <v>0.09</v>
+        <v>0.06</v>
       </c>
       <c r="F39" s="10">
-        <f>0.158*0.9</f>
-        <v>0.14219999999999999</v>
+        <v>5.3100000000000001E-2</v>
       </c>
       <c r="G39" s="10">
         <v>0.3</v>
       </c>
       <c r="H39" s="10">
-        <f t="shared" ref="H39:H40" si="0">7*10^(-11)</f>
-        <v>6.9999999999999991E-11</v>
-      </c>
+        <f>9*10^(-11)</f>
+        <v>8.9999999999999999E-11</v>
+      </c>
+      <c r="I39"/>
+      <c r="J39"/>
+      <c r="K39"/>
+      <c r="L39"/>
+      <c r="M39"/>
+      <c r="N39"/>
+      <c r="O39"/>
+      <c r="P39"/>
+      <c r="Q39"/>
+      <c r="R39"/>
+      <c r="S39"/>
+      <c r="T39"/>
+      <c r="U39"/>
     </row>
     <row r="40" spans="1:16383" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="36" t="s">
@@ -1617,19 +2029,31 @@
         <v>7</v>
       </c>
       <c r="E40" s="11">
-        <v>0.09</v>
+        <v>0.06</v>
       </c>
       <c r="F40" s="10">
-        <f>0.158*0.9</f>
-        <v>0.14219999999999999</v>
+        <v>5.3600000000000002E-2</v>
       </c>
       <c r="G40" s="10">
         <v>0.3</v>
       </c>
       <c r="H40" s="10">
-        <f t="shared" si="0"/>
-        <v>6.9999999999999991E-11</v>
-      </c>
+        <f>9*10^(-11)</f>
+        <v>8.9999999999999999E-11</v>
+      </c>
+      <c r="I40"/>
+      <c r="J40"/>
+      <c r="K40"/>
+      <c r="L40"/>
+      <c r="M40"/>
+      <c r="N40"/>
+      <c r="O40"/>
+      <c r="P40"/>
+      <c r="Q40"/>
+      <c r="R40"/>
+      <c r="S40"/>
+      <c r="T40"/>
+      <c r="U40"/>
     </row>
     <row r="41" spans="1:16383" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="37" t="s">
@@ -1645,18 +2069,30 @@
         <v>5</v>
       </c>
       <c r="E41" s="13">
-        <v>0.09</v>
+        <v>0.06</v>
       </c>
       <c r="F41" s="12">
-        <f>0.164*0.9</f>
-        <v>0.14760000000000001</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="G41" s="12">
         <v>0.3</v>
       </c>
       <c r="H41" s="12">
-        <v>6E-11</v>
-      </c>
+        <v>1E-10</v>
+      </c>
+      <c r="I41"/>
+      <c r="J41"/>
+      <c r="K41"/>
+      <c r="L41"/>
+      <c r="M41"/>
+      <c r="N41"/>
+      <c r="O41"/>
+      <c r="P41"/>
+      <c r="Q41"/>
+      <c r="R41"/>
+      <c r="S41"/>
+      <c r="T41"/>
+      <c r="U41"/>
     </row>
     <row r="42" spans="1:16383" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="37" t="s">
@@ -1672,11 +2108,10 @@
         <v>6</v>
       </c>
       <c r="E42" s="13">
-        <v>0.1</v>
+        <v>0.06</v>
       </c>
       <c r="F42" s="12">
-        <f>0.15*0.9</f>
-        <v>0.13500000000000001</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="G42" s="12">
         <v>0.3</v>
@@ -1684,6 +2119,19 @@
       <c r="H42" s="12">
         <v>1E-10</v>
       </c>
+      <c r="I42"/>
+      <c r="J42"/>
+      <c r="K42"/>
+      <c r="L42"/>
+      <c r="M42"/>
+      <c r="N42"/>
+      <c r="O42"/>
+      <c r="P42"/>
+      <c r="Q42"/>
+      <c r="R42"/>
+      <c r="S42"/>
+      <c r="T42"/>
+      <c r="U42"/>
     </row>
     <row r="43" spans="1:16383" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="37" t="s">
@@ -1699,11 +2147,10 @@
         <v>7</v>
       </c>
       <c r="E43" s="13">
-        <v>0.1</v>
+        <v>0.06</v>
       </c>
       <c r="F43" s="12">
-        <f>0.15*0.9</f>
-        <v>0.13500000000000001</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="G43" s="12">
         <v>0.3</v>
@@ -1711,6 +2158,19 @@
       <c r="H43" s="12">
         <v>1E-10</v>
       </c>
+      <c r="I43"/>
+      <c r="J43"/>
+      <c r="K43"/>
+      <c r="L43"/>
+      <c r="M43"/>
+      <c r="N43"/>
+      <c r="O43"/>
+      <c r="P43"/>
+      <c r="Q43"/>
+      <c r="R43"/>
+      <c r="S43"/>
+      <c r="T43"/>
+      <c r="U43"/>
     </row>
     <row r="44" spans="1:16383" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="38" t="s">
@@ -1726,18 +2186,30 @@
         <v>5</v>
       </c>
       <c r="E44" s="15">
-        <v>0.09</v>
+        <v>0.06</v>
       </c>
       <c r="F44" s="14">
-        <f>5*0.9</f>
-        <v>4.5</v>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="G44" s="14">
-        <v>0.25</v>
+        <v>0.26</v>
       </c>
       <c r="H44" s="14">
-        <v>6E-11</v>
-      </c>
+        <v>1.5E-10</v>
+      </c>
+      <c r="I44"/>
+      <c r="J44"/>
+      <c r="K44"/>
+      <c r="L44"/>
+      <c r="M44"/>
+      <c r="N44"/>
+      <c r="O44"/>
+      <c r="P44"/>
+      <c r="Q44"/>
+      <c r="R44"/>
+      <c r="S44"/>
+      <c r="T44"/>
+      <c r="U44"/>
     </row>
     <row r="45" spans="1:16383" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="38" t="s">
@@ -1753,18 +2225,30 @@
         <v>6</v>
       </c>
       <c r="E45" s="15">
-        <v>0.11</v>
+        <v>0.06</v>
       </c>
       <c r="F45" s="14">
-        <f t="shared" ref="F45:F46" si="1">5*0.9</f>
-        <v>4.5</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="G45" s="14">
-        <v>0.25</v>
+        <v>0.26</v>
       </c>
       <c r="H45" s="14">
-        <v>1E-10</v>
-      </c>
+        <v>1.5E-10</v>
+      </c>
+      <c r="I45"/>
+      <c r="J45"/>
+      <c r="K45"/>
+      <c r="L45"/>
+      <c r="M45"/>
+      <c r="N45"/>
+      <c r="O45"/>
+      <c r="P45"/>
+      <c r="Q45"/>
+      <c r="R45"/>
+      <c r="S45"/>
+      <c r="T45"/>
+      <c r="U45"/>
     </row>
     <row r="46" spans="1:16383" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="38" t="s">
@@ -1780,18 +2264,30 @@
         <v>7</v>
       </c>
       <c r="E46" s="15">
-        <v>0.1</v>
+        <v>0.06</v>
       </c>
       <c r="F46" s="14">
-        <f t="shared" si="1"/>
-        <v>4.5</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="G46" s="14">
-        <v>0.25</v>
+        <v>0.26</v>
       </c>
       <c r="H46" s="14">
-        <v>1E-10</v>
-      </c>
+        <v>1.5E-10</v>
+      </c>
+      <c r="I46"/>
+      <c r="J46"/>
+      <c r="K46"/>
+      <c r="L46"/>
+      <c r="M46"/>
+      <c r="N46"/>
+      <c r="O46"/>
+      <c r="P46"/>
+      <c r="Q46"/>
+      <c r="R46"/>
+      <c r="S46"/>
+      <c r="T46"/>
+      <c r="U46"/>
     </row>
     <row r="47" spans="1:16383" x14ac:dyDescent="0.3">
       <c r="A47" s="32" t="s">
@@ -1807,31 +2303,17 @@
         <v>5</v>
       </c>
       <c r="E47" s="25">
-        <v>0.11</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F47" s="24">
-        <f>0.15*0.9</f>
-        <v>0.13500000000000001</v>
+        <v>9.5000000000000001E-2</v>
       </c>
       <c r="G47" s="24">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
       <c r="H47" s="16">
-        <v>7.0000000000000004E-11</v>
-      </c>
-      <c r="I47" s="16"/>
-      <c r="J47" s="16"/>
-      <c r="K47" s="16"/>
-      <c r="L47" s="16"/>
-      <c r="M47" s="17"/>
-      <c r="N47" s="16"/>
-      <c r="O47" s="16"/>
-      <c r="P47" s="16"/>
-      <c r="Q47" s="16"/>
-      <c r="R47" s="16"/>
-      <c r="S47" s="16"/>
-      <c r="T47" s="16"/>
-      <c r="U47" s="17"/>
+        <v>1E-10</v>
+      </c>
       <c r="V47" s="16"/>
       <c r="W47" s="16"/>
       <c r="X47" s="16"/>
@@ -18209,31 +18691,17 @@
         <v>6</v>
       </c>
       <c r="E48" s="25">
-        <v>0.09</v>
+        <v>0.06</v>
       </c>
       <c r="F48" s="24">
-        <f>0.148*0.9</f>
-        <v>0.13319999999999999</v>
+        <v>0.11</v>
       </c>
       <c r="G48" s="24">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
       <c r="H48" s="16">
-        <v>1E-10</v>
-      </c>
-      <c r="I48" s="16"/>
-      <c r="J48" s="16"/>
-      <c r="K48" s="16"/>
-      <c r="L48" s="16"/>
-      <c r="M48" s="17"/>
-      <c r="N48" s="16"/>
-      <c r="O48" s="16"/>
-      <c r="P48" s="16"/>
-      <c r="Q48" s="16"/>
-      <c r="R48" s="16"/>
-      <c r="S48" s="16"/>
-      <c r="T48" s="16"/>
-      <c r="U48" s="17"/>
+        <v>8.9999999999999999E-11</v>
+      </c>
       <c r="V48" s="16"/>
       <c r="W48" s="16"/>
       <c r="X48" s="16"/>
@@ -34611,31 +35079,17 @@
         <v>7</v>
       </c>
       <c r="E49" s="25">
-        <v>0.09</v>
+        <v>0.06</v>
       </c>
       <c r="F49" s="24">
-        <f>0.148*0.9</f>
-        <v>0.13319999999999999</v>
+        <v>0.109</v>
       </c>
       <c r="G49" s="24">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
       <c r="H49" s="16">
-        <v>1E-10</v>
-      </c>
-      <c r="I49" s="16"/>
-      <c r="J49" s="16"/>
-      <c r="K49" s="16"/>
-      <c r="L49" s="16"/>
-      <c r="M49" s="17"/>
-      <c r="N49" s="16"/>
-      <c r="O49" s="16"/>
-      <c r="P49" s="16"/>
-      <c r="Q49" s="16"/>
-      <c r="R49" s="16"/>
-      <c r="S49" s="16"/>
-      <c r="T49" s="16"/>
-      <c r="U49" s="17"/>
+        <v>8.9999999999999999E-11</v>
+      </c>
       <c r="V49" s="16"/>
       <c r="W49" s="16"/>
       <c r="X49" s="16"/>
@@ -51013,17 +51467,16 @@
         <v>5</v>
       </c>
       <c r="E50" s="19">
-        <v>0.1</v>
+        <v>0.06</v>
       </c>
       <c r="F50" s="18">
-        <f>0.26*0.9</f>
-        <v>0.23400000000000001</v>
+        <v>0.13</v>
       </c>
       <c r="G50" s="18">
         <v>0.3</v>
       </c>
       <c r="H50" s="18">
-        <v>7.0000000000000004E-11</v>
+        <v>8.9999999999999999E-11</v>
       </c>
     </row>
     <row r="51" spans="1:16383" x14ac:dyDescent="0.3">
@@ -51051,9 +51504,6 @@
       <c r="H51" s="18">
         <v>8.9999999999999999E-11</v>
       </c>
-      <c r="I51" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="52" spans="1:16383" x14ac:dyDescent="0.3">
       <c r="A52" s="33" t="s">
@@ -51080,9 +51530,6 @@
       <c r="H52" s="18">
         <v>8.9999999999999999E-11</v>
       </c>
-      <c r="I52" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="53" spans="1:16383" x14ac:dyDescent="0.3">
       <c r="A53" s="34" t="s">
@@ -51101,14 +51548,13 @@
         <v>0.11</v>
       </c>
       <c r="F53" s="20">
-        <f>9*0.9</f>
-        <v>8.1</v>
+        <v>0.2</v>
       </c>
       <c r="G53" s="20">
-        <v>0.25</v>
-      </c>
-      <c r="H53" s="40">
-        <v>7.0000000000000004E-11</v>
+        <v>0.26</v>
+      </c>
+      <c r="H53" s="50">
+        <v>1.5E-10</v>
       </c>
     </row>
     <row r="54" spans="1:16383" x14ac:dyDescent="0.3">
@@ -51128,14 +51574,13 @@
         <v>0.1</v>
       </c>
       <c r="F54" s="20">
-        <f>8*0.9</f>
-        <v>7.2</v>
+        <v>0.18</v>
       </c>
       <c r="G54" s="20">
-        <v>0.25</v>
-      </c>
-      <c r="H54" s="40">
-        <v>1E-10</v>
+        <v>0.26</v>
+      </c>
+      <c r="H54" s="50">
+        <v>1.5E-10</v>
       </c>
     </row>
     <row r="55" spans="1:16383" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -51155,14 +51600,13 @@
         <v>0.1</v>
       </c>
       <c r="F55" s="26">
-        <f>8*0.9</f>
-        <v>7.2</v>
+        <v>0.17</v>
       </c>
       <c r="G55" s="26">
-        <v>0.25</v>
-      </c>
-      <c r="H55" s="43">
-        <v>1E-10</v>
+        <v>0.26</v>
+      </c>
+      <c r="H55" s="51">
+        <v>1.5E-10</v>
       </c>
     </row>
     <row r="56" spans="1:16383" x14ac:dyDescent="0.3">
@@ -51269,6 +51713,20 @@
         <f>0.000000004</f>
         <v>4.0000000000000002E-9</v>
       </c>
+      <c r="I59"/>
+      <c r="J59"/>
+      <c r="K59"/>
+      <c r="L59"/>
+      <c r="M59"/>
+      <c r="N59"/>
+      <c r="O59"/>
+      <c r="P59"/>
+      <c r="Q59"/>
+      <c r="R59"/>
+      <c r="S59"/>
+      <c r="T59"/>
+      <c r="U59"/>
+      <c r="V59"/>
     </row>
     <row r="60" spans="1:16383" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="36" t="s">
@@ -51296,6 +51754,20 @@
         <f>0.000000005*0.8</f>
         <v>4.0000000000000002E-9</v>
       </c>
+      <c r="I60"/>
+      <c r="J60"/>
+      <c r="K60"/>
+      <c r="L60"/>
+      <c r="M60"/>
+      <c r="N60"/>
+      <c r="O60"/>
+      <c r="P60"/>
+      <c r="Q60"/>
+      <c r="R60"/>
+      <c r="S60"/>
+      <c r="T60"/>
+      <c r="U60"/>
+      <c r="V60"/>
     </row>
     <row r="61" spans="1:16383" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="36" t="s">
@@ -51323,6 +51795,20 @@
         <f>0.000000005*0.8</f>
         <v>4.0000000000000002E-9</v>
       </c>
+      <c r="I61"/>
+      <c r="J61"/>
+      <c r="K61"/>
+      <c r="L61"/>
+      <c r="M61"/>
+      <c r="N61"/>
+      <c r="O61"/>
+      <c r="P61"/>
+      <c r="Q61"/>
+      <c r="R61"/>
+      <c r="S61"/>
+      <c r="T61"/>
+      <c r="U61"/>
+      <c r="V61"/>
     </row>
     <row r="62" spans="1:16383" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="37" t="s">
@@ -51349,6 +51835,20 @@
       <c r="H62" s="45">
         <v>4.0000000000000002E-9</v>
       </c>
+      <c r="I62"/>
+      <c r="J62"/>
+      <c r="K62"/>
+      <c r="L62"/>
+      <c r="M62"/>
+      <c r="N62"/>
+      <c r="O62"/>
+      <c r="P62"/>
+      <c r="Q62"/>
+      <c r="R62"/>
+      <c r="S62"/>
+      <c r="T62"/>
+      <c r="U62"/>
+      <c r="V62"/>
     </row>
     <row r="63" spans="1:16383" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="37" t="s">
@@ -51375,6 +51875,20 @@
       <c r="H63" s="45">
         <v>4.0000000000000002E-9</v>
       </c>
+      <c r="I63"/>
+      <c r="J63"/>
+      <c r="K63"/>
+      <c r="L63"/>
+      <c r="M63"/>
+      <c r="N63"/>
+      <c r="O63"/>
+      <c r="P63"/>
+      <c r="Q63"/>
+      <c r="R63"/>
+      <c r="S63"/>
+      <c r="T63"/>
+      <c r="U63"/>
+      <c r="V63"/>
     </row>
     <row r="64" spans="1:16383" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="37" t="s">
@@ -51401,8 +51915,22 @@
       <c r="H64" s="45">
         <v>4.0000000000000002E-9</v>
       </c>
+      <c r="I64"/>
+      <c r="J64"/>
+      <c r="K64"/>
+      <c r="L64"/>
+      <c r="M64"/>
+      <c r="N64"/>
+      <c r="O64"/>
+      <c r="P64"/>
+      <c r="Q64"/>
+      <c r="R64"/>
+      <c r="S64"/>
+      <c r="T64"/>
+      <c r="U64"/>
+      <c r="V64"/>
     </row>
-    <row r="65" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="38" t="s">
         <v>12</v>
       </c>
@@ -51428,8 +51956,22 @@
       <c r="H65" s="46">
         <v>4.0000000000000002E-9</v>
       </c>
+      <c r="I65"/>
+      <c r="J65"/>
+      <c r="K65"/>
+      <c r="L65"/>
+      <c r="M65"/>
+      <c r="N65"/>
+      <c r="O65"/>
+      <c r="P65"/>
+      <c r="Q65"/>
+      <c r="R65"/>
+      <c r="S65"/>
+      <c r="T65"/>
+      <c r="U65"/>
+      <c r="V65"/>
     </row>
-    <row r="66" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66" s="38" t="s">
         <v>12</v>
       </c>
@@ -51446,7 +51988,7 @@
         <v>0.06</v>
       </c>
       <c r="F66" s="14">
-        <f t="shared" ref="F66:F67" si="2">0.00121*0.9</f>
+        <f t="shared" ref="F66:F67" si="0">0.00121*0.9</f>
         <v>1.0889999999999999E-3</v>
       </c>
       <c r="G66" s="14">
@@ -51455,8 +51997,22 @@
       <c r="H66" s="46">
         <v>4.0000000000000002E-9</v>
       </c>
+      <c r="I66"/>
+      <c r="J66"/>
+      <c r="K66"/>
+      <c r="L66"/>
+      <c r="M66"/>
+      <c r="N66"/>
+      <c r="O66"/>
+      <c r="P66"/>
+      <c r="Q66"/>
+      <c r="R66"/>
+      <c r="S66"/>
+      <c r="T66"/>
+      <c r="U66"/>
+      <c r="V66"/>
     </row>
-    <row r="67" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67" s="38" t="s">
         <v>12</v>
       </c>
@@ -51473,7 +52029,7 @@
         <v>0.06</v>
       </c>
       <c r="F67" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1.0889999999999999E-3</v>
       </c>
       <c r="G67" s="14">
@@ -51482,8 +52038,22 @@
       <c r="H67" s="46">
         <v>4.0000000000000002E-9</v>
       </c>
+      <c r="I67"/>
+      <c r="J67"/>
+      <c r="K67"/>
+      <c r="L67"/>
+      <c r="M67"/>
+      <c r="N67"/>
+      <c r="O67"/>
+      <c r="P67"/>
+      <c r="Q67"/>
+      <c r="R67"/>
+      <c r="S67"/>
+      <c r="T67"/>
+      <c r="U67"/>
+      <c r="V67"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A68" s="32" t="s">
         <v>12</v>
       </c>
@@ -51510,7 +52080,7 @@
         <v>3.6E-9</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A69" s="32" t="s">
         <v>12</v>
       </c>
@@ -51533,11 +52103,11 @@
         <v>0.1</v>
       </c>
       <c r="H69" s="47">
-        <f t="shared" ref="H69:H70" si="3">0.0000000045*0.8</f>
+        <f t="shared" ref="H69:H70" si="1">0.0000000045*0.8</f>
         <v>3.6E-9</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A70" s="32" t="s">
         <v>12</v>
       </c>
@@ -51560,11 +52130,11 @@
         <v>0.1</v>
       </c>
       <c r="H70" s="47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>3.6E-9</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A71" s="33" t="s">
         <v>12</v>
       </c>
@@ -51590,7 +52160,7 @@
         <v>3.6E-9</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A72" s="33" t="s">
         <v>12</v>
       </c>
@@ -51616,7 +52186,7 @@
         <v>3.6E-9</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A73" s="33" t="s">
         <v>12</v>
       </c>
@@ -51642,7 +52212,7 @@
         <v>3.6E-9</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A74" s="34" t="s">
         <v>12</v>
       </c>
@@ -51669,7 +52239,7 @@
         <v>3.6E-9</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A75" s="34" t="s">
         <v>12</v>
       </c>
@@ -51686,7 +52256,7 @@
         <v>0.06</v>
       </c>
       <c r="F75" s="20">
-        <f t="shared" ref="F75:F76" si="4">0.00275*0.9</f>
+        <f t="shared" ref="F75:F76" si="2">0.00275*0.9</f>
         <v>2.4749999999999998E-3</v>
       </c>
       <c r="G75" s="20">
@@ -51696,7 +52266,7 @@
         <v>3.6E-9</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="35" t="s">
         <v>12</v>
       </c>
@@ -51713,7 +52283,7 @@
         <v>0.06</v>
       </c>
       <c r="F76" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2.4749999999999998E-3</v>
       </c>
       <c r="G76" s="26">

</xml_diff>